<commit_message>
Removed unnecessary reference files
</commit_message>
<xml_diff>
--- a/project2/servo calibration.xlsx
+++ b/project2/servo calibration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7540"/>
   </bookViews>
   <sheets>
     <sheet name="Right Servo" sheetId="1" r:id="rId1"/>
@@ -2525,16 +2525,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2561,16 +2561,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>60325</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2898,10 +2898,13 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Uploaded final accumulator, right-hand servo PID tuning, & calibrations.
</commit_message>
<xml_diff>
--- a/project2/servo calibration.xlsx
+++ b/project2/servo calibration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="10780" windowHeight="6770" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
   <si>
     <t xml:space="preserve"> Measured T Pass</t>
   </si>
@@ -115,6 +115,12 @@
   <si>
     <t>Steady State:</t>
   </si>
+  <si>
+    <t>T_pass:</t>
+  </si>
+  <si>
+    <t>tau_cl:</t>
+  </si>
 </sst>
 </file>
 
@@ -122,7 +128,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -492,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -555,6 +561,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,20 +606,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -27664,8 +27673,8 @@
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="449034" cy="176972"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -27760,7 +27769,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -27832,8 +27841,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="449034" cy="176972"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -27928,7 +27937,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -28834,34 +28843,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="29"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
     </row>
     <row r="3" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="26"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="33"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
@@ -28907,11 +28916,11 @@
     </row>
     <row r="7" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="8" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
     </row>
     <row r="9" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
@@ -28922,8 +28931,10 @@
         <v>2</v>
       </c>
       <c r="E9" s="3"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23">
+        <v>3.9361330495206586</v>
+      </c>
     </row>
     <row r="10" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="16" t="s">
@@ -28935,8 +28946,10 @@
       <c r="D10" s="5">
         <v>4.1390000000000002</v>
       </c>
-      <c r="F10" s="34"/>
-      <c r="G10" s="35"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="28">
+        <v>4.2841012009485446</v>
+      </c>
     </row>
     <row r="11" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="15" t="s">
@@ -28966,8 +28979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="D7:E7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29040,10 +29053,10 @@
       <c r="B7">
         <v>14</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="26">
         <f>AVERAGE(B2:B98)</f>
         <v>18.402061855670102</v>
       </c>
@@ -29063,6 +29076,13 @@
       <c r="B9">
         <v>15</v>
       </c>
+      <c r="D9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="26">
+        <f>AVERAGE(E22:E25)</f>
+        <v>107.25</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -29079,6 +29099,13 @@
       <c r="B11">
         <v>14</v>
       </c>
+      <c r="D11" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="25">
+        <f>E7/LN(E9)</f>
+        <v>3.9361330495206586</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -29120,7 +29147,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1365</v>
       </c>
@@ -29128,7 +29155,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1366</v>
       </c>
@@ -29136,7 +29163,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1367</v>
       </c>
@@ -29144,7 +29171,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1368</v>
       </c>
@@ -29152,7 +29179,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1369</v>
       </c>
@@ -29160,39 +29187,51 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1370</v>
       </c>
       <c r="B22">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="E22">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1371</v>
       </c>
       <c r="B23">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="E23">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1372</v>
       </c>
       <c r="B24">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="E24">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1373</v>
       </c>
       <c r="B25">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="E25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1374</v>
       </c>
@@ -29200,7 +29239,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1375</v>
       </c>
@@ -29208,7 +29247,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1376</v>
       </c>
@@ -29216,7 +29255,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1377</v>
       </c>
@@ -29224,7 +29263,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1378</v>
       </c>
@@ -29232,7 +29271,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1379</v>
       </c>
@@ -29240,7 +29279,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1380</v>
       </c>
@@ -30468,10 +30507,10 @@
       <c r="B8">
         <v>17</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="37">
+      <c r="E8" s="26">
         <f>AVERAGE(B3:B99)</f>
         <v>17.422680412371133</v>
       </c>
@@ -38206,8 +38245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -38279,10 +38318,10 @@
       <c r="B7">
         <v>20</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="26">
         <f>AVERAGE(B2:B51)</f>
         <v>20.94</v>
       </c>
@@ -38302,6 +38341,13 @@
       <c r="B9">
         <v>21</v>
       </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="27">
+        <f>AVERAGE(E13:E18)</f>
+        <v>132.66666666666666</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -38318,6 +38364,13 @@
       <c r="B11">
         <v>21</v>
       </c>
+      <c r="D11" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="25">
+        <f>E7/LN(E9)</f>
+        <v>4.2841012009485446</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -38334,6 +38387,9 @@
       <c r="B13">
         <v>18</v>
       </c>
+      <c r="E13">
+        <v>125</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -38342,6 +38398,9 @@
       <c r="B14">
         <v>19</v>
       </c>
+      <c r="E14">
+        <v>155</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -38350,6 +38409,9 @@
       <c r="B15">
         <v>19</v>
       </c>
+      <c r="E15">
+        <v>119</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -38358,24 +38420,33 @@
       <c r="B16">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="E16">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1365</v>
       </c>
       <c r="B17">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="E17">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1366</v>
       </c>
       <c r="B18">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="E18">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1367</v>
       </c>
@@ -38383,7 +38454,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1368</v>
       </c>
@@ -38391,7 +38462,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1369</v>
       </c>
@@ -38399,7 +38470,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1370</v>
       </c>
@@ -38407,7 +38478,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1371</v>
       </c>
@@ -38415,7 +38486,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1372</v>
       </c>
@@ -38423,7 +38494,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1373</v>
       </c>
@@ -38431,7 +38502,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1374</v>
       </c>
@@ -38439,7 +38510,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1375</v>
       </c>
@@ -38447,7 +38518,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1376</v>
       </c>
@@ -38455,7 +38526,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1377</v>
       </c>
@@ -38463,7 +38534,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1378</v>
       </c>
@@ -38471,7 +38542,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1379</v>
       </c>
@@ -38479,7 +38550,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1380</v>
       </c>
@@ -39698,10 +39769,10 @@
       <c r="B7">
         <v>21</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="26">
         <f>AVERAGE(B2:B412)</f>
         <v>20.739659367396595</v>
       </c>

</xml_diff>

<commit_message>
Updated servo calibration spreadsheet
</commit_message>
<xml_diff>
--- a/project2/servo calibration.xlsx
+++ b/project2/servo calibration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grafton/Documents/GitHub/me644/project2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grafton/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{932BF78D-A4EC-A040-826D-22508A0C40EE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5524D7D8-4B47-1043-8B68-865683D9BE89}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="LHS B" sheetId="7" r:id="rId3"/>
     <sheet name="RHS A" sheetId="2" r:id="rId4"/>
     <sheet name="RHS B" sheetId="6" r:id="rId5"/>
+    <sheet name="PID" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="lhs_a" localSheetId="1">'LHS A'!$A$1:$B$173</definedName>
@@ -45,15 +46,15 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{AEACFB0E-CE1A-B94B-B908-BD5D1A0EA2DB}" name="lhs-b" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/grafton/Documents/GitHub/me644/project2/calibrations/lhs-b.csv" tab="0" comma="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="lhs-b" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="/Users/grafton/Documents/GitHub/me644/project2/calibrations/lhs-b.csv" tab="0" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="rhs-a1" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="rhs-a1" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr sourceFile="/Users/Grafton/Documents/GitHub/me644/project2/calibrations/rhs-a.csv" tab="0" comma="1">
       <textFields count="2">
         <textField/>
@@ -61,8 +62,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{56BE1187-3B68-6D41-A8AB-64B66CF325F2}" name="rhs-b" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/grafton/Documents/GitHub/me644/project2/calibrations/rhs-b.csv" tab="0" comma="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="rhs-b" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="/Users/grafton/Documents/GitHub/me644/project2/calibrations/rhs-b.csv" tab="0" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t xml:space="preserve"> Measured T Pass</t>
   </si>
@@ -113,15 +114,61 @@
   <si>
     <t>B:</t>
   </si>
+  <si>
+    <t>Steady State:</t>
+  </si>
+  <si>
+    <t>T_pass:</t>
+  </si>
+  <si>
+    <t>tau_cl:</t>
+  </si>
+  <si>
+    <t>(ms)</t>
+  </si>
+  <si>
+    <t>(s)</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Kd</t>
+  </si>
+  <si>
+    <t>PID</t>
+  </si>
+  <si>
+    <t>Kp [Kp/Kd]</t>
+  </si>
+  <si>
+    <t>Ki [Ki/Kd]</t>
+  </si>
+  <si>
+    <t>2% TS</t>
+  </si>
+  <si>
+    <t>ess</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>% OS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,16 +201,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -463,11 +522,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -530,6 +612,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="28" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -560,11 +662,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -27623,13 +27723,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:colOff>146050</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="223779" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <xdr:ext cx="449034" cy="176972"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -27643,8 +27743,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4413250" y="1612900"/>
-              <a:ext cx="223779" cy="172227"/>
+              <a:off x="3956050" y="1689100"/>
+              <a:ext cx="449034" cy="176972"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -27671,6 +27771,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -27701,6 +27802,18 @@
                           </a:rPr>
                           <m:t>𝐶𝐿</m:t>
                         </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>, </m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑅𝐻𝑆</m:t>
+                        </m:r>
                       </m:sub>
                     </m:sSub>
                   </m:oMath>
@@ -27711,7 +27824,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -27725,8 +27838,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4413250" y="1612900"/>
-              <a:ext cx="223779" cy="172227"/>
+              <a:off x="3956050" y="1689100"/>
+              <a:ext cx="449034" cy="176972"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -27753,18 +27866,187 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝜏_</a:t>
+                <a:t>𝜏_(</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝐶𝐿</a:t>
+                <a:t>𝐶𝐿, 𝑅𝐻𝑆)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="449034" cy="176972"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C536977-5950-4FF0-84DB-737A8BA202CE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3956050" y="1511300"/>
+              <a:ext cx="449034" cy="176972"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜏</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐶𝐿</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>, </m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐿𝐻𝑆</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C536977-5950-4FF0-84DB-737A8BA202CE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3956050" y="1511300"/>
+              <a:ext cx="449034" cy="176972"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜏_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐶𝐿, 𝐿𝐻𝑆)</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
@@ -28301,20 +28583,75 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DA1F267-98B0-144C-B63E-3180F7BE4D3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6197600" y="381000"/>
+          <a:ext cx="4927600" cy="4419600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lhs-a" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lhs-b" connectionId="2" xr16:uid="{6C900DF7-3172-6245-B960-1151CE584D27}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lhs-b" connectionId="2" xr16:uid="{00000000-0016-0000-0200-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="rhs-a_1" connectionId="3" xr16:uid="{00000000-0016-0000-0300-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="rhs-a_1" connectionId="3" xr16:uid="{00000000-0016-0000-0300-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="rhs-b" connectionId="4" xr16:uid="{DB2F3844-BCF8-CB47-B668-276B951D7436}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="rhs-b" connectionId="4" xr16:uid="{00000000-0016-0000-0400-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28613,39 +28950,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D525BC1C-EB49-EC40-8F49-77B7D3775B72}">
-  <dimension ref="B1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+    <row r="1" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="29"/>
-    </row>
-    <row r="3" spans="2:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="22" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+    </row>
+    <row r="3" spans="2:8" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="26"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="33"/>
+      <c r="G3" s="36"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
@@ -28665,7 +29002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11">
         <v>1487</v>
       </c>
@@ -28687,15 +29024,21 @@
         <v>1468.5</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="27" t="s">
+    <row r="7" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
-    </row>
-    <row r="9" spans="2:7" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="40"/>
+      <c r="D8" s="41"/>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
       <c r="C9" s="20" t="s">
         <v>6</v>
@@ -28704,12 +29047,16 @@
         <v>2</v>
       </c>
       <c r="E9" s="3"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="32">
-        <v>3.9460000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F9" s="25"/>
+      <c r="G9" s="26">
+        <v>3.9361330495206586</v>
+      </c>
+      <c r="H9" s="27">
+        <f>G9/1000</f>
+        <v>3.9361330495206589E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
         <v>9</v>
       </c>
@@ -28719,8 +29066,16 @@
       <c r="D10" s="5">
         <v>4.1390000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="28"/>
+      <c r="G10" s="29">
+        <v>4.2841012009485446</v>
+      </c>
+      <c r="H10" s="27">
+        <f>G10/1000</f>
+        <v>4.2841012009485445E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
@@ -28729,6 +29084,16 @@
       </c>
       <c r="D11" s="13">
         <v>10.0806</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <f>1/C10</f>
+        <v>0.3143418467583497</v>
+      </c>
+      <c r="D14">
+        <f>1/D10</f>
+        <v>0.24160425223483931</v>
       </c>
     </row>
   </sheetData>
@@ -28739,23 +29104,24 @@
     <mergeCell ref="B8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2581D9B6-B24D-C04E-8CCD-6F4115F4ED06}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E173"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -28820,6 +29186,13 @@
       <c r="B7">
         <v>14</v>
       </c>
+      <c r="D7" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="23">
+        <f>AVERAGE(B2:B98)</f>
+        <v>18.402061855670102</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -28836,6 +29209,13 @@
       <c r="B9">
         <v>15</v>
       </c>
+      <c r="D9" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="23">
+        <f>AVERAGE(E22:E25)</f>
+        <v>107.25</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -28852,6 +29232,13 @@
       <c r="B11">
         <v>14</v>
       </c>
+      <c r="D11" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="22">
+        <f>E7/LN(E9)</f>
+        <v>3.9361330495206586</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -28893,7 +29280,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1365</v>
       </c>
@@ -28901,7 +29288,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1366</v>
       </c>
@@ -28909,7 +29296,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1367</v>
       </c>
@@ -28917,7 +29304,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1368</v>
       </c>
@@ -28925,7 +29312,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1369</v>
       </c>
@@ -28933,39 +29320,51 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1370</v>
       </c>
       <c r="B22">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1371</v>
       </c>
       <c r="B23">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1372</v>
       </c>
       <c r="B24">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1373</v>
       </c>
       <c r="B25">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1374</v>
       </c>
@@ -28973,7 +29372,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1375</v>
       </c>
@@ -28981,7 +29380,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1376</v>
       </c>
@@ -28989,7 +29388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1377</v>
       </c>
@@ -28997,7 +29396,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1378</v>
       </c>
@@ -29005,7 +29404,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1379</v>
       </c>
@@ -29013,7 +29412,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1380</v>
       </c>
@@ -30157,17 +30556,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EFA069-B768-7940-AA18-B0F53884D041}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E973"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D8" sqref="D8:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -30239,6 +30639,13 @@
       </c>
       <c r="B8">
         <v>17</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="23">
+        <f>AVERAGE(B3:B99)</f>
+        <v>17.422680412371133</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -37968,17 +38375,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74A6DA7-5A93-044B-9FE3-F7099E72EAD2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E173"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -38024,8 +38432,8 @@
         <v>7</v>
       </c>
       <c r="E5" s="2">
-        <f>(4.4051+3.8729)/2</f>
-        <v>4.1390000000000002</v>
+        <f>1/((4.4051+3.8729)/2)</f>
+        <v>0.24160425223483931</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -38043,6 +38451,13 @@
       <c r="B7">
         <v>20</v>
       </c>
+      <c r="D7" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="23">
+        <f>AVERAGE(B2:B51)</f>
+        <v>20.94</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -38059,6 +38474,13 @@
       <c r="B9">
         <v>21</v>
       </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="24">
+        <f>AVERAGE(E13:E18)</f>
+        <v>132.66666666666666</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -38075,6 +38497,13 @@
       <c r="B11">
         <v>21</v>
       </c>
+      <c r="D11" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="22">
+        <f>E7/LN(E9)</f>
+        <v>4.2841012009485446</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -38091,6 +38520,9 @@
       <c r="B13">
         <v>18</v>
       </c>
+      <c r="E13">
+        <v>125</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -38099,6 +38531,9 @@
       <c r="B14">
         <v>19</v>
       </c>
+      <c r="E14">
+        <v>155</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -38107,6 +38542,9 @@
       <c r="B15">
         <v>19</v>
       </c>
+      <c r="E15">
+        <v>119</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -38115,24 +38553,33 @@
       <c r="B16">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1365</v>
       </c>
       <c r="B17">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1366</v>
       </c>
       <c r="B18">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1367</v>
       </c>
@@ -38140,7 +38587,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1368</v>
       </c>
@@ -38148,7 +38595,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1369</v>
       </c>
@@ -38156,7 +38603,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1370</v>
       </c>
@@ -38164,7 +38611,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1371</v>
       </c>
@@ -38172,7 +38619,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1372</v>
       </c>
@@ -38180,7 +38627,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1373</v>
       </c>
@@ -38188,7 +38635,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1374</v>
       </c>
@@ -38196,7 +38643,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1375</v>
       </c>
@@ -38204,7 +38651,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1376</v>
       </c>
@@ -38212,7 +38659,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1377</v>
       </c>
@@ -38220,7 +38667,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1378</v>
       </c>
@@ -38228,7 +38675,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1379</v>
       </c>
@@ -38236,7 +38683,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1380</v>
       </c>
@@ -39379,17 +39826,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EEAC89-D4A4-E04B-A2BE-B1AF9ED4BC5C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E973"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -39454,6 +39902,13 @@
       <c r="B7">
         <v>21</v>
       </c>
+      <c r="D7" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="23">
+        <f>AVERAGE(B2:B412)</f>
+        <v>20.739659367396595</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -47181,6 +47636,126 @@
       </c>
       <c r="B973">
         <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>2.5832999999999997E-4</v>
+      </c>
+      <c r="C2">
+        <f>3190*B2</f>
+        <v>0.82407269999999988</v>
+      </c>
+      <c r="D2">
+        <f>2540000*B2</f>
+        <v>656.15819999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="30">
+        <v>8.4541000000000004</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>5.5100000000000001E-3</v>
+      </c>
+      <c r="F3">
+        <v>0.67100000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>73.820999999999998</v>
+      </c>
+      <c r="C4">
+        <f>B4*72.76</f>
+        <v>5371.2159600000005</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>0.67342999999999997</v>
+      </c>
+      <c r="C5">
+        <v>472</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>2.3E-2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="31">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>